<commit_message>
Update log4j dependencies and add database source file
This commit modifies the pom.xml file to update the log4j dependencies by defining the version in the properties section and using that property in the dependencies list. Therefore, we need to update the version only at one place in future. Also, a new XML was added that defines a PostgreSQL database source. In addition, Playwright browser launch options were updated to launch in headless mode.
</commit_message>
<xml_diff>
--- a/src/test/resources/ConnectionsACP.xlsx
+++ b/src/test/resources/ConnectionsACP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalst/IdeaProjects/SaveATrainPlaywrith/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9079149-5193-3146-9915-8B5849B13FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1B2BAF-F8CB-9B42-B3A5-58A1AA687CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17400" xr2:uid="{800225BC-0EDC-F14A-9F21-CBE6997CEC23}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:C7572"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,7 +439,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>45379.292361111111</v>
+        <v>45412.292361111111</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -450,7 +450,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1">
-        <v>45379.292361111111</v>
+        <v>45412.292361111111</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add enrichment API tests and update dependencies
New tests for the Rail Enrichment API were added, and changes were made to existing tests. The codebase was updated to include the RailEnrichmentAPIProductPage. Dependencies in pom.xml file were also updated - Apache Commons Compress was bumped from version 1.26.0 to 1.26.1.
</commit_message>
<xml_diff>
--- a/src/test/resources/ConnectionsACP.xlsx
+++ b/src/test/resources/ConnectionsACP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalst/IdeaProjects/SaveATrainPlaywrith/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1B2BAF-F8CB-9B42-B3A5-58A1AA687CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DBC325-3A9D-EA43-B8ED-78D6362ECE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17400" xr2:uid="{800225BC-0EDC-F14A-9F21-CBE6997CEC23}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:C7572"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,7 +439,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>45412.292361111111</v>
+        <v>45442.292361111111</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -450,7 +450,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1">
-        <v>45412.292361111111</v>
+        <v>45442.292361111111</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Refactor MainPage.java and update methods
The MainPage class has been significantly refactored. Variable declarations have been made private, and hard-coded strings have been replaced with static final variables, where appropriate, for cleaner code. Several methods in the class have also been updated to use these variables instead of strings. In the SaveATrainE2EACPTests class, a line has been commented out. This commit improves code readability, consistency, and maintainability.
</commit_message>
<xml_diff>
--- a/src/test/resources/ConnectionsACP.xlsx
+++ b/src/test/resources/ConnectionsACP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalst/IdeaProjects/SaveATrainPlaywrith/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DBC325-3A9D-EA43-B8ED-78D6362ECE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C010287-73B8-7440-BFE8-4B109360CDBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17400" xr2:uid="{800225BC-0EDC-F14A-9F21-CBE6997CEC23}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:C7572"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,7 +439,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>45442.292361111111</v>
+        <v>45471.292361111111</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -450,7 +450,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1">
-        <v>45442.292361111111</v>
+        <v>45471.292361111111</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update test execution order and selector changes
The commit reorder the test execution sequence to perform search before inputting origin and destination stations. Also, changed the input selectors to match the new UI structure. Furthermore, test for headless browser execution has been set to true and an unnecessary hover action has been commented out.
</commit_message>
<xml_diff>
--- a/src/test/resources/ConnectionsACP.xlsx
+++ b/src/test/resources/ConnectionsACP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalst/IdeaProjects/SaveATrainPlaywrith/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C010287-73B8-7440-BFE8-4B109360CDBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C443660E-4B7D-1643-B76E-DF0AC711C7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17400" xr2:uid="{800225BC-0EDC-F14A-9F21-CBE6997CEC23}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:C7572"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,7 +439,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>45471.292361111111</v>
+        <v>45502.292361111111</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -450,7 +450,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1">
-        <v>45471.292361111111</v>
+        <v>45502.292361111111</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>